<commit_message>
tambahan unit kantor tapi belum full
</commit_message>
<xml_diff>
--- a/uploads/template_pegawai.xlsx
+++ b/uploads/template_pegawai.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MyBook Hype AMD\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\laragon\www\SKI-BRK\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A53523A8-0B36-48D5-9790-A161B6C3ACA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D155ED1C-4E86-430C-AEF5-55D54AB3F75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{771B09B1-6B79-440A-B52C-E27A1A492057}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10890" xr2:uid="{771B09B1-6B79-440A-B52C-E27A1A492057}"/>
   </bookViews>
   <sheets>
     <sheet name="Lembar1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Jabatan</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>Unit Kerja</t>
   </si>
 </sst>
 </file>
@@ -104,7 +107,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -400,19 +403,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9348FA11-D9D0-446B-97A6-DA6E341322FC}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.36328125" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -423,9 +430,12 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>